<commit_message>
Updated fuel prices for coal to use *imported* coal prices, which aligns with other research from NREL and confirmed by IEA, which shows that Mexico imports the vast majority of coal. This brought coal dispatch in line with historical data. Then I noticed that HFO was flagged as a peaker and getting guaranteed dispatch at a 50% CF. I turned off the flag as a peaker, which dropped the dispatch. I am comparing to the report from NREL referenced in Monday.com and the results are very close to what they have for historical dispatch, so I think we are in good shape on start year dispatch and fuel prices. I'll do a bit more digging on projections.
</commit_message>
<xml_diff>
--- a/InputData/elec/BPaFF/Boolean Peaking and Flexibility Flags.xlsx
+++ b/InputData/elec/BPaFF/Boolean Peaking and Flexibility Flags.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anaxolt/Google Drive/2021/D.Development/TARGET_eps-us-3.2.1/InputData/elec/BPaFF/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\Mexico\Models\eps-mexico\InputData\elec\BPaFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC860AF-A1DA-6E4A-81F3-467E0747FB1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B969A6B8-171E-4180-9627-55366D48E04A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="500" windowWidth="23960" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -550,23 +550,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -574,116 +574,116 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -701,19 +701,21 @@
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
@@ -721,7 +723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -729,7 +731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -737,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -745,7 +747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -753,7 +755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -761,7 +763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -769,7 +771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -777,7 +779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -785,7 +787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -793,7 +795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -801,7 +803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -810,7 +812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -819,25 +821,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
       <c r="B15">
-        <f>B11</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
       <c r="B16">
-        <f>B11</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -860,17 +860,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
@@ -878,7 +878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -886,7 +886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -894,7 +894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -902,7 +902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -910,7 +910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -918,7 +918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -926,7 +926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -934,7 +934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -942,7 +942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -950,7 +950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -958,7 +958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -967,7 +967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -976,7 +976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -985,7 +985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -994,7 +994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>

</xml_diff>